<commit_message>
Extend backward to 15 Feb
</commit_message>
<xml_diff>
--- a/output/italy.xlsx
+++ b/output/italy.xlsx
@@ -6,7 +6,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="01Mar-15May" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="15Feb-15May" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="1Feb-4Feb" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="5Feb-11Feb" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="12Feb-18Feb" sheetId="4" state="visible" r:id="rId4"/>
@@ -63,79 +63,79 @@
     <t xml:space="preserve">All ages</t>
   </si>
   <si>
-    <t xml:space="preserve">179929</t>
+    <t xml:space="preserve">208320</t>
   </si>
   <si>
     <t xml:space="preserve">Less than 60</t>
   </si>
   <si>
-    <t xml:space="preserve">9863</t>
+    <t xml:space="preserve">11719</t>
   </si>
   <si>
     <t xml:space="preserve">60-69</t>
   </si>
   <si>
-    <t xml:space="preserve">18702</t>
+    <t xml:space="preserve">21703</t>
   </si>
   <si>
     <t xml:space="preserve">70-79</t>
   </si>
   <si>
-    <t xml:space="preserve">35717</t>
+    <t xml:space="preserve">41198</t>
   </si>
   <si>
     <t xml:space="preserve">80-89</t>
   </si>
   <si>
-    <t xml:space="preserve">71415</t>
+    <t xml:space="preserve">82259</t>
   </si>
   <si>
     <t xml:space="preserve">90 and older</t>
   </si>
   <si>
-    <t xml:space="preserve">46768</t>
+    <t xml:space="preserve">54392</t>
   </si>
   <si>
     <t xml:space="preserve">Males</t>
   </si>
   <si>
-    <t xml:space="preserve">88108</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6288</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12347</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22065</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34975</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14260</t>
+    <t xml:space="preserve">101568</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7478</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25314</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40136</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16522</t>
   </si>
   <si>
     <t xml:space="preserve">Females</t>
   </si>
   <si>
-    <t xml:space="preserve">91824</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3576</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6356</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13654</t>
-  </si>
-  <si>
-    <t xml:space="preserve">36445</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32508</t>
+    <t xml:space="preserve">106754</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4242</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7469</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15886</t>
+  </si>
+  <si>
+    <t xml:space="preserve">42128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37870</t>
   </si>
   <si>
     <t xml:space="preserve">7792</t>
@@ -1338,22 +1338,22 @@
         <v>11</v>
       </c>
       <c r="D2" t="n">
-        <v>47245</v>
+        <v>47490</v>
       </c>
       <c r="E2" t="n">
-        <v>44147</v>
+        <v>43984</v>
       </c>
       <c r="F2" t="n">
-        <v>49868</v>
+        <v>50362</v>
       </c>
       <c r="G2" t="n">
-        <v>35.6</v>
+        <v>29.5</v>
       </c>
       <c r="H2" t="n">
-        <v>32.5</v>
+        <v>26.8</v>
       </c>
       <c r="I2" t="n">
-        <v>38.3</v>
+        <v>31.9</v>
       </c>
     </row>
     <row r="3">
@@ -1367,22 +1367,22 @@
         <v>13</v>
       </c>
       <c r="D3" t="n">
-        <v>1069</v>
+        <v>1088</v>
       </c>
       <c r="E3" t="n">
-        <v>-356</v>
+        <v>-426</v>
       </c>
       <c r="F3" t="n">
-        <v>2123</v>
+        <v>2209</v>
       </c>
       <c r="G3" t="n">
-        <v>12.2</v>
+        <v>10.2</v>
       </c>
       <c r="H3" t="n">
         <v>-3.5</v>
       </c>
       <c r="I3" t="n">
-        <v>27.4</v>
+        <v>23.2</v>
       </c>
     </row>
     <row r="4">
@@ -1396,22 +1396,22 @@
         <v>15</v>
       </c>
       <c r="D4" t="n">
-        <v>4338</v>
+        <v>4386</v>
       </c>
       <c r="E4" t="n">
-        <v>3283</v>
+        <v>3286</v>
       </c>
       <c r="F4" t="n">
-        <v>5077</v>
+        <v>5157</v>
       </c>
       <c r="G4" t="n">
-        <v>30.2</v>
+        <v>25.3</v>
       </c>
       <c r="H4" t="n">
-        <v>21.3</v>
+        <v>17.8</v>
       </c>
       <c r="I4" t="n">
-        <v>37.3</v>
+        <v>31.2</v>
       </c>
     </row>
     <row r="5">
@@ -1425,22 +1425,22 @@
         <v>17</v>
       </c>
       <c r="D5" t="n">
-        <v>10522</v>
+        <v>10614</v>
       </c>
       <c r="E5" t="n">
-        <v>8215</v>
+        <v>8256</v>
       </c>
       <c r="F5" t="n">
-        <v>12369</v>
+        <v>12524</v>
       </c>
       <c r="G5" t="n">
-        <v>41.8</v>
+        <v>34.7</v>
       </c>
       <c r="H5" t="n">
-        <v>29.9</v>
+        <v>25.1</v>
       </c>
       <c r="I5" t="n">
-        <v>53</v>
+        <v>43.7</v>
       </c>
     </row>
     <row r="6">
@@ -1454,22 +1454,22 @@
         <v>19</v>
       </c>
       <c r="D6" t="n">
-        <v>20584</v>
+        <v>20674</v>
       </c>
       <c r="E6" t="n">
-        <v>19264</v>
+        <v>19377</v>
       </c>
       <c r="F6" t="n">
-        <v>21328</v>
+        <v>21387</v>
       </c>
       <c r="G6" t="n">
-        <v>40.5</v>
+        <v>33.6</v>
       </c>
       <c r="H6" t="n">
-        <v>36.9</v>
+        <v>30.8</v>
       </c>
       <c r="I6" t="n">
-        <v>42.6</v>
+        <v>35.1</v>
       </c>
     </row>
     <row r="7">
@@ -1483,22 +1483,22 @@
         <v>21</v>
       </c>
       <c r="D7" t="n">
-        <v>12075</v>
+        <v>12114</v>
       </c>
       <c r="E7" t="n">
-        <v>11006</v>
+        <v>10877</v>
       </c>
       <c r="F7" t="n">
-        <v>12699</v>
+        <v>12858</v>
       </c>
       <c r="G7" t="n">
-        <v>34.8</v>
+        <v>28.7</v>
       </c>
       <c r="H7" t="n">
-        <v>30.8</v>
+        <v>25</v>
       </c>
       <c r="I7" t="n">
-        <v>37.3</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8">
@@ -1512,22 +1512,22 @@
         <v>23</v>
       </c>
       <c r="D8" t="n">
-        <v>24517</v>
+        <v>24655</v>
       </c>
       <c r="E8" t="n">
-        <v>22566</v>
+        <v>22604</v>
       </c>
       <c r="F8" t="n">
-        <v>25922</v>
+        <v>26215</v>
       </c>
       <c r="G8" t="n">
-        <v>38.6</v>
+        <v>32.1</v>
       </c>
       <c r="H8" t="n">
-        <v>34.4</v>
+        <v>28.6</v>
       </c>
       <c r="I8" t="n">
-        <v>41.7</v>
+        <v>34.8</v>
       </c>
     </row>
     <row r="9">
@@ -1541,22 +1541,22 @@
         <v>24</v>
       </c>
       <c r="D9" t="n">
-        <v>884</v>
+        <v>935</v>
       </c>
       <c r="E9" t="n">
-        <v>226</v>
+        <v>246</v>
       </c>
       <c r="F9" t="n">
-        <v>1267</v>
+        <v>1342</v>
       </c>
       <c r="G9" t="n">
-        <v>16.4</v>
+        <v>14.3</v>
       </c>
       <c r="H9" t="n">
-        <v>3.7</v>
+        <v>3.4</v>
       </c>
       <c r="I9" t="n">
-        <v>25.2</v>
+        <v>21.9</v>
       </c>
     </row>
     <row r="10">
@@ -1570,22 +1570,22 @@
         <v>25</v>
       </c>
       <c r="D10" t="n">
-        <v>3439</v>
+        <v>3505</v>
       </c>
       <c r="E10" t="n">
-        <v>2621</v>
+        <v>2646</v>
       </c>
       <c r="F10" t="n">
-        <v>3909</v>
+        <v>4006</v>
       </c>
       <c r="G10" t="n">
-        <v>38.6</v>
+        <v>32.7</v>
       </c>
       <c r="H10" t="n">
-        <v>26.9</v>
+        <v>22.8</v>
       </c>
       <c r="I10" t="n">
-        <v>46.3</v>
+        <v>39.2</v>
       </c>
     </row>
     <row r="11">
@@ -1599,22 +1599,22 @@
         <v>26</v>
       </c>
       <c r="D11" t="n">
-        <v>7173</v>
+        <v>7219</v>
       </c>
       <c r="E11" t="n">
-        <v>5849</v>
+        <v>5646</v>
       </c>
       <c r="F11" t="n">
-        <v>8161</v>
+        <v>8364</v>
       </c>
       <c r="G11" t="n">
-        <v>48.2</v>
+        <v>39.9</v>
       </c>
       <c r="H11" t="n">
-        <v>36.1</v>
+        <v>28.7</v>
       </c>
       <c r="I11" t="n">
-        <v>58.7</v>
+        <v>49.3</v>
       </c>
     </row>
     <row r="12">
@@ -1628,22 +1628,22 @@
         <v>27</v>
       </c>
       <c r="D12" t="n">
-        <v>10754</v>
+        <v>10855</v>
       </c>
       <c r="E12" t="n">
-        <v>9368</v>
+        <v>9410</v>
       </c>
       <c r="F12" t="n">
-        <v>11624</v>
+        <v>11716</v>
       </c>
       <c r="G12" t="n">
-        <v>44.4</v>
+        <v>37.1</v>
       </c>
       <c r="H12" t="n">
-        <v>36.6</v>
+        <v>30.6</v>
       </c>
       <c r="I12" t="n">
-        <v>49.8</v>
+        <v>41.2</v>
       </c>
     </row>
     <row r="13">
@@ -1657,22 +1657,22 @@
         <v>28</v>
       </c>
       <c r="D13" t="n">
-        <v>3625</v>
+        <v>3623</v>
       </c>
       <c r="E13" t="n">
-        <v>2883</v>
+        <v>2849</v>
       </c>
       <c r="F13" t="n">
-        <v>4092</v>
+        <v>4055</v>
       </c>
       <c r="G13" t="n">
-        <v>34.1</v>
+        <v>28.1</v>
       </c>
       <c r="H13" t="n">
-        <v>25.3</v>
+        <v>20.8</v>
       </c>
       <c r="I13" t="n">
-        <v>40.2</v>
+        <v>32.5</v>
       </c>
     </row>
     <row r="14">
@@ -1686,22 +1686,22 @@
         <v>30</v>
       </c>
       <c r="D14" t="n">
-        <v>23001</v>
+        <v>23125</v>
       </c>
       <c r="E14" t="n">
-        <v>21044</v>
+        <v>20997</v>
       </c>
       <c r="F14" t="n">
-        <v>24401</v>
+        <v>24609</v>
       </c>
       <c r="G14" t="n">
-        <v>33.4</v>
+        <v>27.7</v>
       </c>
       <c r="H14" t="n">
-        <v>29.7</v>
+        <v>24.5</v>
       </c>
       <c r="I14" t="n">
-        <v>36.2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15">
@@ -1715,22 +1715,22 @@
         <v>31</v>
       </c>
       <c r="D15" t="n">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="E15" t="n">
-        <v>-193</v>
+        <v>-242</v>
       </c>
       <c r="F15" t="n">
-        <v>852</v>
+        <v>882</v>
       </c>
       <c r="G15" t="n">
-        <v>13.6</v>
+        <v>11.3</v>
       </c>
       <c r="H15" t="n">
-        <v>-5.1</v>
+        <v>-5.4</v>
       </c>
       <c r="I15" t="n">
-        <v>31.3</v>
+        <v>26.2</v>
       </c>
     </row>
     <row r="16">
@@ -1744,22 +1744,22 @@
         <v>32</v>
       </c>
       <c r="D16" t="n">
-        <v>1129</v>
+        <v>1154</v>
       </c>
       <c r="E16" t="n">
-        <v>713</v>
+        <v>739</v>
       </c>
       <c r="F16" t="n">
-        <v>1364</v>
+        <v>1388</v>
       </c>
       <c r="G16" t="n">
-        <v>21.6</v>
+        <v>18.3</v>
       </c>
       <c r="H16" t="n">
-        <v>12.6</v>
+        <v>11</v>
       </c>
       <c r="I16" t="n">
-        <v>27.3</v>
+        <v>22.8</v>
       </c>
     </row>
     <row r="17">
@@ -1773,22 +1773,22 @@
         <v>33</v>
       </c>
       <c r="D17" t="n">
-        <v>3583</v>
+        <v>3676</v>
       </c>
       <c r="E17" t="n">
-        <v>2363</v>
+        <v>2399</v>
       </c>
       <c r="F17" t="n">
-        <v>4319</v>
+        <v>4438</v>
       </c>
       <c r="G17" t="n">
-        <v>35.6</v>
+        <v>30.1</v>
       </c>
       <c r="H17" t="n">
-        <v>20.9</v>
+        <v>17.8</v>
       </c>
       <c r="I17" t="n">
-        <v>46.3</v>
+        <v>38.8</v>
       </c>
     </row>
     <row r="18">
@@ -1802,22 +1802,22 @@
         <v>34</v>
       </c>
       <c r="D18" t="n">
-        <v>10077</v>
+        <v>10090</v>
       </c>
       <c r="E18" t="n">
-        <v>9235</v>
+        <v>9181</v>
       </c>
       <c r="F18" t="n">
-        <v>10567</v>
+        <v>10629</v>
       </c>
       <c r="G18" t="n">
-        <v>38.2</v>
+        <v>31.5</v>
       </c>
       <c r="H18" t="n">
-        <v>33.9</v>
+        <v>27.9</v>
       </c>
       <c r="I18" t="n">
-        <v>40.8</v>
+        <v>33.7</v>
       </c>
     </row>
     <row r="19">
@@ -1831,22 +1831,22 @@
         <v>35</v>
       </c>
       <c r="D19" t="n">
-        <v>8717</v>
+        <v>8806</v>
       </c>
       <c r="E19" t="n">
-        <v>7721</v>
+        <v>7590</v>
       </c>
       <c r="F19" t="n">
-        <v>9275</v>
+        <v>9536</v>
       </c>
       <c r="G19" t="n">
-        <v>36.6</v>
+        <v>30.3</v>
       </c>
       <c r="H19" t="n">
-        <v>31.1</v>
+        <v>25.1</v>
       </c>
       <c r="I19" t="n">
-        <v>39.9</v>
+        <v>33.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>